<commit_message>
added 7.1 test case 1
i added the first test case, both on the SRS and the excel
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6321BD-BEE4-4E6B-B826-94382D0B0471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{0F6321BD-BEE4-4E6B-B826-94382D0B0471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D9BA167-EB63-4FC8-B63E-ED02D63F23EE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -80,6 +80,39 @@
   </si>
   <si>
     <t>TesterK</t>
+  </si>
+  <si>
+    <t>Philip Revak</t>
+  </si>
+  <si>
+    <t>CreateAccount_1</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Website is open in a suported browser</t>
+  </si>
+  <si>
+    <t>Verify that the proccess of account creation functions properly</t>
+  </si>
+  <si>
+    <t>Account is successfully created</t>
+  </si>
+  <si>
+    <t>1. Navigate to the create account page
+2.Enter a valid username in the username box.
+3. Enter a valid password in the password box.
+4. Click the create account button.</t>
+  </si>
+  <si>
+    <t>Not yet tested</t>
+  </si>
+  <si>
+    <t>Not Executed</t>
   </si>
 </sst>
 </file>
@@ -117,7 +150,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +166,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -164,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -178,6 +217,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +538,7 @@
     <col min="6" max="6" width="34.5546875" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.109375" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -580,6 +620,38 @@
         <v>20</v>
       </c>
     </row>
+    <row r="4" spans="1:10" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>

</xml_diff>

<commit_message>
added test case 5 to the excel
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{0F6321BD-BEE4-4E6B-B826-94382D0B0471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D9BA167-EB63-4FC8-B63E-ED02D63F23EE}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{0F6321BD-BEE4-4E6B-B826-94382D0B0471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DE72C59-BF6B-4EC5-A75B-E1D4E9DE24E3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -50,36 +50,7 @@
     <t>Pre-requisites</t>
   </si>
   <si>
-    <t>GoogleSearch_1</t>
-  </si>
-  <si>
-    <t>Search_Bar_Module</t>
-  </si>
-  <si>
     <t>P0</t>
-  </si>
-  <si>
-    <t>Verify that when a user writes a search term and presses enter, search results should be displayed</t>
-  </si>
-  <si>
-    <t>Browser is launched</t>
-  </si>
-  <si>
-    <t>1. Write the url - http://google.com in the browser's URL bar and press enter.
-2. Once google.com is launched, write the search term - "Apple" in the google search bar.
-3. Press enter.</t>
-  </si>
-  <si>
-    <t>Search results related to 'apple' should be displayed</t>
-  </si>
-  <si>
-    <t>Search results with 'apple' keyword are displayed</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>TesterK</t>
   </si>
   <si>
     <t>Philip Revak</t>
@@ -113,6 +84,23 @@
   </si>
   <si>
     <t>Not Executed</t>
+  </si>
+  <si>
+    <t>createOrder_1</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>verify that the createOrder function works correctly</t>
+  </si>
+  <si>
+    <t>1. Initalize the Order class.
+2. Call the createOrder(userID, showTimeID, seatNumbers) function with valid userID, showTimeID, and avalible seatNumbers.
+3. repeat the call with invalid values for userID, showTimeID, and unavalible seatNumbers</t>
+  </si>
+  <si>
+    <t>An order is corectly created for valid inputs and an error describing the correct invalid input is returned for invalid inputs</t>
   </si>
 </sst>
 </file>
@@ -150,7 +138,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,12 +148,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -203,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -217,7 +199,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -233,6 +214,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -522,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,68 +573,68 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="69.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test case 6 to the excel and updated the SRS
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{0F6321BD-BEE4-4E6B-B826-94382D0B0471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DE72C59-BF6B-4EC5-A75B-E1D4E9DE24E3}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{0F6321BD-BEE4-4E6B-B826-94382D0B0471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{909B324F-C9F0-4AF9-96A4-7E18DF6B39E4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3588" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseTemplate" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Test Executed By</t>
-  </si>
-  <si>
-    <t>Test Case Template</t>
   </si>
   <si>
     <t>Pre-requisites</t>
@@ -86,13 +83,7 @@
     <t>Not Executed</t>
   </si>
   <si>
-    <t>createOrder_1</t>
-  </si>
-  <si>
     <t>Order</t>
-  </si>
-  <si>
-    <t>verify that the createOrder function works correctly</t>
   </si>
   <si>
     <t>1. Initalize the Order class.
@@ -101,13 +92,152 @@
   </si>
   <si>
     <t>An order is corectly created for valid inputs and an error describing the correct invalid input is returned for invalid inputs</t>
+  </si>
+  <si>
+    <t>CreateOrder_1</t>
+  </si>
+  <si>
+    <t>SystemTest_1</t>
+  </si>
+  <si>
+    <t>Full System</t>
+  </si>
+  <si>
+    <t>Verify that the createOrder function works correctly</t>
+  </si>
+  <si>
+    <t>Verify the complete functionality of the system from login to checkout</t>
+  </si>
+  <si>
+    <t>1. Sign in with a valid username and password
+2. Select a movie and a theauter
+3. Select seats
+4. Enter payment information and complete Payment
+5. Verify the recipt is correct, the seat is booked, and the payment was recived</t>
+  </si>
+  <si>
+    <t>All steps are completed without errors, the receipt  is correct, payment was received, the seat is properly booked, transaction information is saved properly</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>Login Auth_2</t>
+  </si>
+  <si>
+    <t>User Login Module</t>
+  </si>
+  <si>
+    <t>Verify that valid users can log in and invalid attempts are rejected</t>
+  </si>
+  <si>
+    <t>Website is open in a suported browser. At least one user account exists</t>
+  </si>
+  <si>
+    <t>1. Navigate to the login page.
+2.Enter registered email and valid password.
+3. Click Login.
+4.Repeat with wrong password or email.</t>
+  </si>
+  <si>
+    <t>Valid login redirects to dashboard, invalid password displays "Incorrect password."</t>
+  </si>
+  <si>
+    <t>Anthony Diego</t>
+  </si>
+  <si>
+    <t>SeatSelect_3</t>
+  </si>
+  <si>
+    <t>Seat Selection Module</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>Verify that users can select available seats and that double-booking is prevented.</t>
+  </si>
+  <si>
+    <t>Movie and showtime are available in the database</t>
+  </si>
+  <si>
+    <t>1. Select a theater and movie.
+2. Choose available seats.
+3. Proceed to checkout.
+4. Attempt to reserve the same seats from another browser.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seats shows as "Reserved", second user sees seat unavailable. </t>
+  </si>
+  <si>
+    <t>Payment_4</t>
+  </si>
+  <si>
+    <t>Payment Gateway Module</t>
+  </si>
+  <si>
+    <t>Verify that ticket purchases and payments process correctly</t>
+  </si>
+  <si>
+    <t>Valid seat selection and user info entered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Proceed to payment page
+2. Enter valid credit card info.
+3. Click Purchase.
+4. Repeat with invalid or expired card. </t>
+  </si>
+  <si>
+    <t>Valid card completes payment and sends email receipt, invalid card shows "Payment Failed."</t>
+  </si>
+  <si>
+    <t>Refund_5</t>
+  </si>
+  <si>
+    <t>Admin Dashboard</t>
+  </si>
+  <si>
+    <t>Verify that only admins can refund user orders.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin account logged in, at least one completed order exists. </t>
+  </si>
+  <si>
+    <t>1. Log in as admin.
+2. Open Orders page.
+3. Select an order and click Refund.
+4. Confirm refund request.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refund processed, order marked "Cancelled", customer receives refund email. </t>
+  </si>
+  <si>
+    <t>PasswordReset_6</t>
+  </si>
+  <si>
+    <t>User Account Module</t>
+  </si>
+  <si>
+    <t>Verify that users can successfully reset their password through the email verification process</t>
+  </si>
+  <si>
+    <t>User account with a valid registered email exists.</t>
+  </si>
+  <si>
+    <t>1. Go to the Forgot Password page.
+2. Enter registered email address.
+3. Check email inbox for verification code.
+4. Enter verification code and new password on reset form.                          5. Try logging in using the new password.</t>
+  </si>
+  <si>
+    <t>Password reset email received, new password accepted upon login.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +267,18 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -158,7 +300,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -181,11 +323,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -198,6 +399,24 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -214,10 +433,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -507,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,7 +744,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -555,7 +770,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
@@ -575,66 +790,258 @@
     </row>
     <row r="3" spans="1:10" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="H7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="4" t="s">
+    </row>
+    <row r="8" spans="1:10" ht="138" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>12</v>
+      <c r="J8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="81" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="58.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="81" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added remaining test cases & updated case IDs
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{0F6321BD-BEE4-4E6B-B826-94382D0B0471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{909B324F-C9F0-4AF9-96A4-7E18DF6B39E4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BC27B25-7752-474C-BA4E-EB287654DE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3588" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24555" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseTemplate" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -92,12 +92,6 @@
   </si>
   <si>
     <t>An order is corectly created for valid inputs and an error describing the correct invalid input is returned for invalid inputs</t>
-  </si>
-  <si>
-    <t>CreateOrder_1</t>
-  </si>
-  <si>
-    <t>SystemTest_1</t>
   </si>
   <si>
     <t>Full System</t>
@@ -122,9 +116,6 @@
     <t>Test Cases</t>
   </si>
   <si>
-    <t>Login Auth_2</t>
-  </si>
-  <si>
     <t>User Login Module</t>
   </si>
   <si>
@@ -146,9 +137,6 @@
     <t>Anthony Diego</t>
   </si>
   <si>
-    <t>SeatSelect_3</t>
-  </si>
-  <si>
     <t>Seat Selection Module</t>
   </si>
   <si>
@@ -170,9 +158,6 @@
     <t xml:space="preserve">Seats shows as "Reserved", second user sees seat unavailable. </t>
   </si>
   <si>
-    <t>Payment_4</t>
-  </si>
-  <si>
     <t>Payment Gateway Module</t>
   </si>
   <si>
@@ -191,9 +176,6 @@
     <t>Valid card completes payment and sends email receipt, invalid card shows "Payment Failed."</t>
   </si>
   <si>
-    <t>Refund_5</t>
-  </si>
-  <si>
     <t>Admin Dashboard</t>
   </si>
   <si>
@@ -212,9 +194,6 @@
     <t xml:space="preserve">Refund processed, order marked "Cancelled", customer receives refund email. </t>
   </si>
   <si>
-    <t>PasswordReset_6</t>
-  </si>
-  <si>
     <t>User Account Module</t>
   </si>
   <si>
@@ -231,6 +210,73 @@
   </si>
   <si>
     <t>Password reset email received, new password accepted upon login.</t>
+  </si>
+  <si>
+    <t>CreateOrder_2</t>
+  </si>
+  <si>
+    <t>SystemTest_3</t>
+  </si>
+  <si>
+    <t>Login Auth_4</t>
+  </si>
+  <si>
+    <t>SeatSelect_5</t>
+  </si>
+  <si>
+    <t>Payment_6</t>
+  </si>
+  <si>
+    <t>Refund_7</t>
+  </si>
+  <si>
+    <t>PasswordReset_8</t>
+  </si>
+  <si>
+    <t>PromoCode_9</t>
+  </si>
+  <si>
+    <t>Payment Gateway</t>
+  </si>
+  <si>
+    <t>Verify that valid promo codes correctly apply discounts correctly and invalid codes display an error.</t>
+  </si>
+  <si>
+    <t>User has selected tickets and reached the payment page</t>
+  </si>
+  <si>
+    <t>1. On the payment page, enter a valid promo code.
+2. Verify that the total cost updates to the correct amount after the discount is applied.
+3. Enter an invalid promo code.
+4. Try to complete the payment.</t>
+  </si>
+  <si>
+    <t>After entering the valid promo code, the total cust shows the correct amount after the discount is applied and the invalid promo code displays an error.</t>
+  </si>
+  <si>
+    <t>James Shumate</t>
+  </si>
+  <si>
+    <t>PromoCode_10</t>
+  </si>
+  <si>
+    <t>User and Payment Gateway</t>
+  </si>
+  <si>
+    <t>Verify integration between User and Payment modules, ensuring purchases are correctly displayed in the user's purchase history.</t>
+  </si>
+  <si>
+    <t>User is logged in to a user account.</t>
+  </si>
+  <si>
+    <t>1. Log in as a user.
+2. Select a theater, then movie, then select seats.
+3. Complete the purchase.
+4. Navigate to the user's purchase history.
+5. Confirm that the purchase appears with correct details.</t>
+  </si>
+  <si>
+    <t>The purchase correctly appears in the user's purchase history. The data is consistent between Payment and User modules.</t>
   </si>
 </sst>
 </file>
@@ -397,9 +443,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -417,6 +460,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,41 +768,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -788,7 +834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="69.599999999999994" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="80.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -820,228 +866,292 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="92.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="4" spans="1:10" ht="114" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="136.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="G5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="91.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>11</v>
+      <c r="J7" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="138" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
+    <row r="8" spans="1:10" ht="91.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="D8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>11</v>
+      <c r="J8" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="81" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>32</v>
+    <row r="9" spans="1:10" ht="80.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>14</v>
+        <v>47</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>35</v>
+        <v>48</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="13" t="s">
-        <v>38</v>
+      <c r="J9" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="58.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="9" t="s">
+    <row r="10" spans="1:10" ht="91.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="9" t="s">
-        <v>38</v>
+      <c r="J10" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="92.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="H11" s="9" t="s">
+    <row r="11" spans="1:10" ht="125.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="9" t="s">
-        <v>38</v>
+      <c r="J11" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="81" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" s="9" t="s">
+    <row r="12" spans="1:10" ht="125.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="92.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>38</v>
+      <c r="J12" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed PromoCode_10 to UserOrderIntegration_10
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BC27B25-7752-474C-BA4E-EB287654DE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF4CF17-1864-47FD-A651-F382084845DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24555" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseTemplate" sheetId="1" r:id="rId1"/>
@@ -257,9 +257,6 @@
     <t>James Shumate</t>
   </si>
   <si>
-    <t>PromoCode_10</t>
-  </si>
-  <si>
     <t>User and Payment Gateway</t>
   </si>
   <si>
@@ -277,6 +274,9 @@
   </si>
   <si>
     <t>The purchase correctly appears in the user's purchase history. The data is consistent between Payment and User modules.</t>
+  </si>
+  <si>
+    <t>UserOrderIntegration_10</t>
   </si>
 </sst>
 </file>
@@ -771,7 +771,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,25 +1124,25 @@
     </row>
     <row r="12" spans="1:10" ht="125.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>19</v>

</xml_diff>